<commit_message>
Commit of following modifications :
- output file name
- storing files names
- security net in case of null response
- added EMC dates in Synthese_fileEMC
-prompt construction
</commit_message>
<xml_diff>
--- a/Synthese_fileEMC.xlsx
+++ b/Synthese_fileEMC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bessec\Recherche\Articles\article29\ChatGPT\EMC_BdF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC2383AA-3ABF-4B55-BD01-B9BE7E08DA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{131650A6-5A39-430C-B5AA-B9ED74A20FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{25461E42-27EB-457B-B6F5-ECD54AB476A0}"/>
   </bookViews>
@@ -417,7 +417,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="258">
   <si>
     <t>format court (ancien)</t>
   </si>
@@ -1149,13 +1149,55 @@
   </si>
   <si>
     <t>EMC_12_2024</t>
+  </si>
+  <si>
+    <t>EMC_1_2025</t>
+  </si>
+  <si>
+    <t>2025T1</t>
+  </si>
+  <si>
+    <t>EMC_2_2025</t>
+  </si>
+  <si>
+    <t>EMC_3_2025</t>
+  </si>
+  <si>
+    <t>EMC_4_2025</t>
+  </si>
+  <si>
+    <t>2025T2</t>
+  </si>
+  <si>
+    <t>EMC_5_2025</t>
+  </si>
+  <si>
+    <t>EMC_6_2025</t>
+  </si>
+  <si>
+    <t>EMC_7_2025</t>
+  </si>
+  <si>
+    <t>2025T3</t>
+  </si>
+  <si>
+    <t>EMC_8_2025</t>
+  </si>
+  <si>
+    <t>EMC_9_2025</t>
+  </si>
+  <si>
+    <t>EMC_10_2025</t>
+  </si>
+  <si>
+    <t>2025T4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1166,14 +1208,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1248,13 +1282,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1571,11 +1605,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF4B610-5B33-430E-BCA3-7CA060183EF3}">
-  <dimension ref="A1:D195"/>
+  <dimension ref="A1:D207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B128" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F145" sqref="F145"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C180" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C189" sqref="C189"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -1585,7 +1619,8 @@
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="20.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="6"/>
+    <col min="5" max="5" width="44.42578125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1735,7 +1770,7 @@
       <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1882,7 +1917,7 @@
       <c r="A26" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="9"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="1" t="s">
         <v>4</v>
       </c>
@@ -2029,7 +2064,7 @@
       <c r="A39" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="9"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="1" t="s">
         <v>4</v>
       </c>
@@ -2176,7 +2211,7 @@
       <c r="A52" t="s">
         <v>67</v>
       </c>
-      <c r="B52" s="9"/>
+      <c r="B52" s="8"/>
       <c r="C52" s="1" t="s">
         <v>4</v>
       </c>
@@ -2323,7 +2358,7 @@
       <c r="A65" t="s">
         <v>83</v>
       </c>
-      <c r="B65" s="9"/>
+      <c r="B65" s="8"/>
       <c r="C65" s="1" t="s">
         <v>4</v>
       </c>
@@ -2492,7 +2527,7 @@
       <c r="A78" t="s">
         <v>99</v>
       </c>
-      <c r="B78" s="8">
+      <c r="B78" s="7">
         <v>42381</v>
       </c>
       <c r="C78" s="1" t="s">
@@ -2663,7 +2698,7 @@
       <c r="A91" t="s">
         <v>115</v>
       </c>
-      <c r="B91" s="8">
+      <c r="B91" s="7">
         <v>42744</v>
       </c>
       <c r="C91" s="1" t="s">
@@ -2834,7 +2869,7 @@
       <c r="A104" t="s">
         <v>131</v>
       </c>
-      <c r="B104" s="8">
+      <c r="B104" s="7">
         <v>43111</v>
       </c>
       <c r="C104" s="1" t="s">
@@ -3005,7 +3040,7 @@
       <c r="A117" t="s">
         <v>147</v>
       </c>
-      <c r="B117" s="8">
+      <c r="B117" s="7">
         <v>43476</v>
       </c>
       <c r="C117" s="1" t="s">
@@ -3176,7 +3211,7 @@
       <c r="A130" t="s">
         <v>163</v>
       </c>
-      <c r="B130" s="8">
+      <c r="B130" s="7">
         <v>43840</v>
       </c>
       <c r="C130" s="1" t="s">
@@ -3853,15 +3888,15 @@
         <v>231</v>
       </c>
     </row>
-    <row r="189" spans="1:4">
+    <row r="189" spans="1:4" ht="15">
       <c r="A189" t="s">
         <v>235</v>
       </c>
       <c r="B189" s="2">
         <v>45483</v>
       </c>
-      <c r="C189" s="7">
-        <v>45482</v>
+      <c r="C189" s="9">
+        <v>45483</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>231</v>
@@ -3947,6 +3982,119 @@
       </c>
       <c r="D195" s="1" t="s">
         <v>241</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="D196" s="1"/>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" t="s">
+        <v>244</v>
+      </c>
+      <c r="C198" s="2">
+        <v>45699</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" t="s">
+        <v>246</v>
+      </c>
+      <c r="C199" s="2">
+        <v>45728</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" t="s">
+        <v>247</v>
+      </c>
+      <c r="C200" s="2">
+        <v>45755</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" t="s">
+        <v>248</v>
+      </c>
+      <c r="C201" s="2">
+        <v>45790</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" t="s">
+        <v>250</v>
+      </c>
+      <c r="C202" s="2">
+        <v>45819</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" t="s">
+        <v>251</v>
+      </c>
+      <c r="C203" s="2">
+        <v>45847</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" t="s">
+        <v>252</v>
+      </c>
+      <c r="C204" s="2">
+        <v>45880</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" t="s">
+        <v>254</v>
+      </c>
+      <c r="C205" s="2">
+        <v>45909</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206" t="s">
+        <v>255</v>
+      </c>
+      <c r="C206" s="2">
+        <v>45939</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207" t="s">
+        <v>256</v>
+      </c>
+      <c r="C207" s="2">
+        <v>45973</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Adding a file to compute each model's MAE/RMSE and compare them
- Deleting a wrong date in Script_fileEMC
</commit_message>
<xml_diff>
--- a/Synthese_fileEMC.xlsx
+++ b/Synthese_fileEMC.xlsx
@@ -1,413 +1,422 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bessec\Recherche\Articles\article29\ChatGPT\EMC_BdF\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{131650A6-5A39-430C-B5AA-B9ED74A20FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{25461E42-27EB-457B-B6F5-ECD54AB476A0}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Marie Bessec</author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="B179" authorId="0" shapeId="0" xr:uid="{9C07311D-2A96-4474-8704-9D4F0BFEFCC4}">
+    <comment authorId="0" ref="B179">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages</t>
+          <t xml:space="preserve">17 pages</t>
         </r>
       </text>
     </comment>
-    <comment ref="B180" authorId="0" shapeId="0" xr:uid="{49023505-BC9A-453C-B6E6-A384C7199FC6}">
+    <comment authorId="0" ref="B180">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages</t>
+          <t xml:space="preserve">17 pages</t>
         </r>
       </text>
     </comment>
-    <comment ref="B181" authorId="0" shapeId="0" xr:uid="{65E6894F-6DF3-4B19-9473-6F64A467D369}">
+    <comment authorId="0" ref="B181">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages</t>
+          <t xml:space="preserve">17 pages</t>
         </r>
       </text>
     </comment>
-    <comment ref="B182" authorId="0" shapeId="0" xr:uid="{FC00E3DC-6F4C-47F0-819A-BE2B8040C702}">
+    <comment authorId="0" ref="B182">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages</t>
+          <t xml:space="preserve">17 pages</t>
         </r>
       </text>
     </comment>
-    <comment ref="B184" authorId="0" shapeId="0" xr:uid="{9FB98D6E-5CD9-4AFD-8D7E-373250320291}">
+    <comment authorId="0" ref="B184">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages
+          <t xml:space="preserve">17 pages
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B185" authorId="0" shapeId="0" xr:uid="{6864A501-7425-44BE-8943-121C4746D302}">
+    <comment authorId="0" ref="B185">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages
+          <t xml:space="preserve">17 pages
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B186" authorId="0" shapeId="0" xr:uid="{29D9D8AA-6A42-4896-B664-24778F7B12D0}">
+    <comment authorId="0" ref="B186">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages
+          <t xml:space="preserve">17 pages
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B187" authorId="0" shapeId="0" xr:uid="{D9DFF767-1E56-4584-A26C-4F1E53881DAD}">
+    <comment authorId="0" ref="B187">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages
+          <t xml:space="preserve">17 pages
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B188" authorId="0" shapeId="0" xr:uid="{95C6A76D-C951-4EB6-B73C-044DAD84CB2F}">
+    <comment authorId="0" ref="B188">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages
+          <t xml:space="preserve">17 pages
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B189" authorId="0" shapeId="0" xr:uid="{D6460A3F-E0B1-4B89-AFB1-98B5B6BF8BFA}">
+    <comment authorId="0" ref="B189">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages
+          <t xml:space="preserve">17 pages
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B190" authorId="0" shapeId="0" xr:uid="{B44E0189-2E6D-4E9F-969E-248B7381681A}">
+    <comment authorId="0" ref="B190">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages
+          <t xml:space="preserve">17 pages
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B192" authorId="0" shapeId="0" xr:uid="{E3ED0FCE-D113-46FC-8A63-90F87D31CA56}">
+    <comment authorId="0" ref="B192">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages
+          <t xml:space="preserve">17 pages
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B193" authorId="0" shapeId="0" xr:uid="{172A11CA-6EA5-4C7C-98C6-6F03ED2D72EE}">
+    <comment authorId="0" ref="B193">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages
+          <t xml:space="preserve">17 pages
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B194" authorId="0" shapeId="0" xr:uid="{2E4053CB-59EC-45D1-877B-6C1E342CE2B0}">
+    <comment authorId="0" ref="B194">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages
+          <t xml:space="preserve">17 pages
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B195" authorId="0" shapeId="0" xr:uid="{7C262807-30E6-4C7C-9567-C6D5C81B6622}">
+    <comment authorId="0" ref="B195">
       <text>
         <r>
           <rPr>
-            <b/>
+            <b val="true"/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Marie Bessec:</t>
+          <t xml:space="preserve">Marie Bessec:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-17 pages
+          <t xml:space="preserve">17 pages
 </t>
         </r>
       </text>
@@ -1196,40 +1205,61 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="DD\-MMM\-YY" numFmtId="165"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1241,19 +1271,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -1261,369 +1291,169 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="15" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="15" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="5" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFC000"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF4B610-5B33-430E-BCA3-7CA060183EF3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C180" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C189" sqref="C189"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="bottomRight" state="frozen" topLeftCell="C138" xSplit="2" ySplit="1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="C1" activeCellId="0" pane="topRight" sqref="C1"/>
+      <selection activeCell="A138" activeCellId="0" pane="bottomLeft" sqref="A138"/>
+      <selection activeCell="B144" activeCellId="0" pane="bottomRight" sqref="B144"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="44.42578125" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="20.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.9948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="44.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="2" width="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1634,11 +1464,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1646,11 +1476,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1658,11 +1488,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1670,11 +1500,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1682,11 +1512,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1694,11 +1524,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1706,11 +1536,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1718,11 +1548,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="9">
+      <c r="A9" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1730,11 +1560,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="10">
+      <c r="A10" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1742,11 +1572,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1754,11 +1584,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="12">
+      <c r="A12" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1766,11 +1596,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="13">
+      <c r="A13" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1778,14 +1608,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="14">
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="15">
+      <c r="A15" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1793,11 +1625,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="16">
+      <c r="A16" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="1" t="s">
         <v>4</v>
       </c>
@@ -1805,11 +1637,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="17">
+      <c r="A17" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="3"/>
       <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1817,11 +1649,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="18">
+      <c r="A18" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
@@ -1829,11 +1661,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="19">
+      <c r="A19" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="3"/>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1841,11 +1673,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="20">
+      <c r="A20" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="3"/>
       <c r="C20" s="1" t="s">
         <v>4</v>
       </c>
@@ -1853,11 +1685,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="21">
+      <c r="A21" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="3"/>
       <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1865,11 +1697,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="22">
+      <c r="A22" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="3"/>
       <c r="C22" s="1" t="s">
         <v>4</v>
       </c>
@@ -1877,11 +1709,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="23">
+      <c r="A23" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="4"/>
+      <c r="B23" s="3"/>
       <c r="C23" s="1" t="s">
         <v>4</v>
       </c>
@@ -1889,11 +1721,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="24">
+      <c r="A24" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="3"/>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1901,11 +1733,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="25">
+      <c r="A25" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="4"/>
+      <c r="B25" s="3"/>
       <c r="C25" s="1" t="s">
         <v>4</v>
       </c>
@@ -1913,11 +1745,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="26">
+      <c r="A26" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="4"/>
       <c r="C26" s="1" t="s">
         <v>4</v>
       </c>
@@ -1925,14 +1757,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="27">
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="28">
+      <c r="A28" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="4"/>
+      <c r="B28" s="3"/>
       <c r="C28" s="1" t="s">
         <v>4</v>
       </c>
@@ -1940,11 +1774,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="29">
+      <c r="A29" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="4"/>
+      <c r="B29" s="3"/>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
@@ -1952,11 +1786,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="30">
+      <c r="A30" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="3"/>
       <c r="C30" s="1" t="s">
         <v>4</v>
       </c>
@@ -1964,11 +1798,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="31">
+      <c r="A31" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="3"/>
       <c r="C31" s="1" t="s">
         <v>4</v>
       </c>
@@ -1976,11 +1810,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="32">
+      <c r="A32" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B32" s="3"/>
       <c r="C32" s="1" t="s">
         <v>4</v>
       </c>
@@ -1988,11 +1822,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="33">
+      <c r="A33" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="4"/>
+      <c r="B33" s="3"/>
       <c r="C33" s="1" t="s">
         <v>4</v>
       </c>
@@ -2000,11 +1834,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="34">
+      <c r="A34" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="4"/>
+      <c r="B34" s="3"/>
       <c r="C34" s="1" t="s">
         <v>4</v>
       </c>
@@ -2012,11 +1846,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="35">
+      <c r="A35" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="4"/>
+      <c r="B35" s="3"/>
       <c r="C35" s="1" t="s">
         <v>4</v>
       </c>
@@ -2024,11 +1858,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="36">
+      <c r="A36" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="4"/>
+      <c r="B36" s="3"/>
       <c r="C36" s="1" t="s">
         <v>4</v>
       </c>
@@ -2036,11 +1870,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="37">
+      <c r="A37" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="4"/>
+      <c r="B37" s="3"/>
       <c r="C37" s="1" t="s">
         <v>4</v>
       </c>
@@ -2048,11 +1882,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="38">
+      <c r="A38" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="4"/>
+      <c r="B38" s="3"/>
       <c r="C38" s="1" t="s">
         <v>4</v>
       </c>
@@ -2060,11 +1894,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="39">
+      <c r="A39" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="8"/>
+      <c r="B39" s="4"/>
       <c r="C39" s="1" t="s">
         <v>4</v>
       </c>
@@ -2072,14 +1906,16 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="40">
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="41">
+      <c r="A41" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="4"/>
+      <c r="B41" s="3"/>
       <c r="C41" s="1" t="s">
         <v>4</v>
       </c>
@@ -2087,11 +1923,11 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="42">
+      <c r="A42" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="4"/>
+      <c r="B42" s="3"/>
       <c r="C42" s="1" t="s">
         <v>4</v>
       </c>
@@ -2099,11 +1935,11 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="43">
+      <c r="A43" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="4"/>
+      <c r="B43" s="3"/>
       <c r="C43" s="1" t="s">
         <v>4</v>
       </c>
@@ -2111,11 +1947,11 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="44">
+      <c r="A44" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B44" s="4"/>
+      <c r="B44" s="3"/>
       <c r="C44" s="1" t="s">
         <v>4</v>
       </c>
@@ -2123,11 +1959,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="45">
+      <c r="A45" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="4"/>
+      <c r="B45" s="3"/>
       <c r="C45" s="1" t="s">
         <v>4</v>
       </c>
@@ -2135,11 +1971,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="46">
+      <c r="A46" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B46" s="4"/>
+      <c r="B46" s="3"/>
       <c r="C46" s="1" t="s">
         <v>4</v>
       </c>
@@ -2147,11 +1983,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="47">
+      <c r="A47" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B47" s="4"/>
+      <c r="B47" s="3"/>
       <c r="C47" s="1" t="s">
         <v>4</v>
       </c>
@@ -2159,11 +1995,11 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="48">
+      <c r="A48" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="4"/>
+      <c r="B48" s="3"/>
       <c r="C48" s="1" t="s">
         <v>4</v>
       </c>
@@ -2171,11 +2007,11 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="49">
+      <c r="A49" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B49" s="4"/>
+      <c r="B49" s="3"/>
       <c r="C49" s="1" t="s">
         <v>4</v>
       </c>
@@ -2183,11 +2019,11 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="50">
+      <c r="A50" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="4"/>
+      <c r="B50" s="3"/>
       <c r="C50" s="1" t="s">
         <v>4</v>
       </c>
@@ -2195,11 +2031,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="51">
+      <c r="A51" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B51" s="4"/>
+      <c r="B51" s="3"/>
       <c r="C51" s="1" t="s">
         <v>4</v>
       </c>
@@ -2207,11 +2043,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="52">
+      <c r="A52" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B52" s="8"/>
+      <c r="B52" s="4"/>
       <c r="C52" s="1" t="s">
         <v>4</v>
       </c>
@@ -2219,14 +2055,16 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="53">
+      <c r="B53" s="0"/>
+      <c r="C53" s="0"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="54">
+      <c r="A54" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B54" s="4"/>
+      <c r="B54" s="3"/>
       <c r="C54" s="1" t="s">
         <v>4</v>
       </c>
@@ -2234,11 +2072,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="55">
+      <c r="A55" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B55" s="4"/>
+      <c r="B55" s="3"/>
       <c r="C55" s="1" t="s">
         <v>4</v>
       </c>
@@ -2246,11 +2084,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="56">
+      <c r="A56" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B56" s="4"/>
+      <c r="B56" s="3"/>
       <c r="C56" s="1" t="s">
         <v>4</v>
       </c>
@@ -2258,11 +2096,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="57">
+      <c r="A57" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B57" s="4"/>
+      <c r="B57" s="3"/>
       <c r="C57" s="1" t="s">
         <v>4</v>
       </c>
@@ -2270,11 +2108,11 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="58">
+      <c r="A58" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="B58" s="4"/>
+      <c r="B58" s="3"/>
       <c r="C58" s="1" t="s">
         <v>4</v>
       </c>
@@ -2282,11 +2120,11 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="59">
+      <c r="A59" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B59" s="4"/>
+      <c r="B59" s="3"/>
       <c r="C59" s="1" t="s">
         <v>4</v>
       </c>
@@ -2294,11 +2132,11 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="60">
+      <c r="A60" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B60" s="4"/>
+      <c r="B60" s="3"/>
       <c r="C60" s="1" t="s">
         <v>4</v>
       </c>
@@ -2306,11 +2144,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="61">
+      <c r="A61" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B61" s="4"/>
+      <c r="B61" s="3"/>
       <c r="C61" s="1" t="s">
         <v>4</v>
       </c>
@@ -2318,11 +2156,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
-      <c r="A62" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="62">
+      <c r="A62" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="B62" s="4"/>
+      <c r="B62" s="3"/>
       <c r="C62" s="1" t="s">
         <v>4</v>
       </c>
@@ -2330,11 +2168,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="63">
+      <c r="A63" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B63" s="4"/>
+      <c r="B63" s="3"/>
       <c r="C63" s="1" t="s">
         <v>4</v>
       </c>
@@ -2342,11 +2180,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
-      <c r="A64" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="64">
+      <c r="A64" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B64" s="4"/>
+      <c r="B64" s="3"/>
       <c r="C64" s="1" t="s">
         <v>4</v>
       </c>
@@ -2354,11 +2192,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="65">
+      <c r="A65" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="B65" s="8"/>
+      <c r="B65" s="4"/>
       <c r="C65" s="1" t="s">
         <v>4</v>
       </c>
@@ -2366,14 +2204,16 @@
         <v>81</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="66">
+      <c r="B66" s="0"/>
+      <c r="C66" s="0"/>
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="1:4">
-      <c r="A67" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="67">
+      <c r="A67" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="5" t="n">
         <v>42044</v>
       </c>
       <c r="C67" s="1" t="s">
@@ -2383,11 +2223,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
-      <c r="A68" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="68">
+      <c r="A68" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="5" t="n">
         <v>42072</v>
       </c>
       <c r="C68" s="1" t="s">
@@ -2397,11 +2237,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
-      <c r="A69" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="69">
+      <c r="A69" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="5" t="n">
         <v>42103</v>
       </c>
       <c r="C69" s="1" t="s">
@@ -2411,11 +2251,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
-      <c r="A70" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="70">
+      <c r="A70" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="5" t="n">
         <v>42136</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -2425,11 +2265,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
-      <c r="A71" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="71">
+      <c r="A71" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="5" t="n">
         <v>42163</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -2439,11 +2279,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
-      <c r="A72" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="72">
+      <c r="A72" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="5" t="n">
         <v>42193</v>
       </c>
       <c r="C72" s="1" t="s">
@@ -2453,11 +2293,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
-      <c r="A73" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="73">
+      <c r="A73" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="5" t="n">
         <v>42226</v>
       </c>
       <c r="C73" s="1" t="s">
@@ -2467,11 +2307,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
-      <c r="A74" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="74">
+      <c r="A74" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="5" t="n">
         <v>42255</v>
       </c>
       <c r="C74" s="1" t="s">
@@ -2481,11 +2321,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
-      <c r="A75" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="75">
+      <c r="A75" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="5" t="n">
         <v>42285</v>
       </c>
       <c r="C75" s="1" t="s">
@@ -2495,11 +2335,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
-      <c r="A76" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="76">
+      <c r="A76" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="5" t="n">
         <v>42317</v>
       </c>
       <c r="C76" s="1" t="s">
@@ -2509,11 +2349,11 @@
         <v>97</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
-      <c r="A77" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="77">
+      <c r="A77" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="5" t="n">
         <v>42346</v>
       </c>
       <c r="C77" s="1" t="s">
@@ -2523,11 +2363,11 @@
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
-      <c r="A78" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="78">
+      <c r="A78" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="B78" s="7">
+      <c r="B78" s="6" t="n">
         <v>42381</v>
       </c>
       <c r="C78" s="1" t="s">
@@ -2537,14 +2377,16 @@
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="79">
+      <c r="B79" s="0"/>
+      <c r="C79" s="0"/>
       <c r="D79" s="1"/>
     </row>
-    <row r="80" spans="1:4">
-      <c r="A80" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="80">
+      <c r="A80" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="5" t="n">
         <v>42408</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -2554,11 +2396,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
-      <c r="A81" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="81">
+      <c r="A81" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="5" t="n">
         <v>42438</v>
       </c>
       <c r="C81" s="1" t="s">
@@ -2568,11 +2410,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
-      <c r="A82" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="82">
+      <c r="A82" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="5" t="n">
         <v>42468</v>
       </c>
       <c r="C82" s="1" t="s">
@@ -2582,11 +2424,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
-      <c r="A83" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="83">
+      <c r="A83" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="5" t="n">
         <v>42500</v>
       </c>
       <c r="C83" s="1" t="s">
@@ -2596,11 +2438,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
-      <c r="A84" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="84">
+      <c r="A84" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84" s="5" t="n">
         <v>42529</v>
       </c>
       <c r="C84" s="1" t="s">
@@ -2610,11 +2452,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
-      <c r="A85" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="85">
+      <c r="A85" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85" s="5" t="n">
         <v>42562</v>
       </c>
       <c r="C85" s="1" t="s">
@@ -2624,11 +2466,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
-      <c r="A86" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="86">
+      <c r="A86" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86" s="5" t="n">
         <v>42590</v>
       </c>
       <c r="C86" s="1" t="s">
@@ -2638,11 +2480,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="87">
+      <c r="A87" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="5" t="n">
         <v>42621</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -2652,11 +2494,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
-      <c r="A88" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="88">
+      <c r="A88" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="5" t="n">
         <v>42653</v>
       </c>
       <c r="C88" s="1" t="s">
@@ -2666,11 +2508,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
-      <c r="A89" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="89">
+      <c r="A89" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="5" t="n">
         <v>42683</v>
       </c>
       <c r="C89" s="1" t="s">
@@ -2680,11 +2522,11 @@
         <v>113</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
-      <c r="A90" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="90">
+      <c r="A90" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="5" t="n">
         <v>42712</v>
       </c>
       <c r="C90" s="1" t="s">
@@ -2694,11 +2536,11 @@
         <v>113</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
-      <c r="A91" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="91">
+      <c r="A91" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="B91" s="7">
+      <c r="B91" s="6" t="n">
         <v>42744</v>
       </c>
       <c r="C91" s="1" t="s">
@@ -2708,14 +2550,16 @@
         <v>113</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="92">
+      <c r="B92" s="0"/>
+      <c r="C92" s="0"/>
       <c r="D92" s="1"/>
     </row>
-    <row r="93" spans="1:4">
-      <c r="A93" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="93">
+      <c r="A93" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93" s="5" t="n">
         <v>42774</v>
       </c>
       <c r="C93" s="1" t="s">
@@ -2725,11 +2569,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
-      <c r="A94" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="94">
+      <c r="A94" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94" s="5" t="n">
         <v>42803</v>
       </c>
       <c r="C94" s="1" t="s">
@@ -2739,11 +2583,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
-      <c r="A95" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="95">
+      <c r="A95" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95" s="5" t="n">
         <v>42835</v>
       </c>
       <c r="C95" s="1" t="s">
@@ -2753,11 +2597,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
-      <c r="A96" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="96">
+      <c r="A96" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B96" s="5" t="n">
         <v>42864</v>
       </c>
       <c r="C96" s="1" t="s">
@@ -2767,11 +2611,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
-      <c r="A97" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="97">
+      <c r="A97" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B97" s="5" t="n">
         <v>42898</v>
       </c>
       <c r="C97" s="1" t="s">
@@ -2781,11 +2625,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
-      <c r="A98" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="98">
+      <c r="A98" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98" s="5" t="n">
         <v>42926</v>
       </c>
       <c r="C98" s="1" t="s">
@@ -2795,11 +2639,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
-      <c r="A99" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="99">
+      <c r="A99" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B99" s="5" t="n">
         <v>42956</v>
       </c>
       <c r="C99" s="1" t="s">
@@ -2809,11 +2653,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
-      <c r="A100" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="100">
+      <c r="A100" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100" s="5" t="n">
         <v>42989</v>
       </c>
       <c r="C100" s="1" t="s">
@@ -2823,11 +2667,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
-      <c r="A101" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="101">
+      <c r="A101" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B101" s="5" t="n">
         <v>43017</v>
       </c>
       <c r="C101" s="1" t="s">
@@ -2837,11 +2681,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
-      <c r="A102" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="102">
+      <c r="A102" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="B102" s="2">
+      <c r="B102" s="5" t="n">
         <v>43048</v>
       </c>
       <c r="C102" s="1" t="s">
@@ -2851,11 +2695,11 @@
         <v>129</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
-      <c r="A103" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="103">
+      <c r="A103" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B103" s="2">
+      <c r="B103" s="5" t="n">
         <v>43080</v>
       </c>
       <c r="C103" s="1" t="s">
@@ -2865,11 +2709,11 @@
         <v>129</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
-      <c r="A104" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="104">
+      <c r="A104" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="B104" s="7">
+      <c r="B104" s="6" t="n">
         <v>43111</v>
       </c>
       <c r="C104" s="1" t="s">
@@ -2879,14 +2723,16 @@
         <v>129</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="105">
+      <c r="B105" s="0"/>
+      <c r="C105" s="0"/>
       <c r="D105" s="1"/>
     </row>
-    <row r="106" spans="1:4">
-      <c r="A106" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="106">
+      <c r="A106" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="B106" s="2">
+      <c r="B106" s="5" t="n">
         <v>43139</v>
       </c>
       <c r="C106" s="1" t="s">
@@ -2896,11 +2742,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
-      <c r="A107" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="107">
+      <c r="A107" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B107" s="2">
+      <c r="B107" s="5" t="n">
         <v>43167</v>
       </c>
       <c r="C107" s="1" t="s">
@@ -2910,11 +2756,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
-      <c r="A108" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="108">
+      <c r="A108" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B108" s="2">
+      <c r="B108" s="5" t="n">
         <v>43201</v>
       </c>
       <c r="C108" s="1" t="s">
@@ -2924,11 +2770,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
-      <c r="A109" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="109">
+      <c r="A109" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="B109" s="2">
+      <c r="B109" s="5" t="n">
         <v>43234</v>
       </c>
       <c r="C109" s="1" t="s">
@@ -2938,11 +2784,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
-      <c r="A110" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="110">
+      <c r="A110" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="B110" s="2">
+      <c r="B110" s="5" t="n">
         <v>43262</v>
       </c>
       <c r="C110" s="1" t="s">
@@ -2952,11 +2798,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
-      <c r="A111" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="111">
+      <c r="A111" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="B111" s="2">
+      <c r="B111" s="5" t="n">
         <v>43290</v>
       </c>
       <c r="C111" s="1" t="s">
@@ -2966,11 +2812,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
-      <c r="A112" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="112">
+      <c r="A112" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="B112" s="2">
+      <c r="B112" s="5" t="n">
         <v>43320</v>
       </c>
       <c r="C112" s="1" t="s">
@@ -2980,11 +2826,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
-      <c r="A113" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="113">
+      <c r="A113" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B113" s="2">
+      <c r="B113" s="5" t="n">
         <v>43353</v>
       </c>
       <c r="C113" s="1" t="s">
@@ -2994,11 +2840,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
-      <c r="A114" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="114">
+      <c r="A114" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B114" s="2">
+      <c r="B114" s="5" t="n">
         <v>43381</v>
       </c>
       <c r="C114" s="1" t="s">
@@ -3008,11 +2854,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
-      <c r="A115" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="115">
+      <c r="A115" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B115" s="2">
+      <c r="B115" s="5" t="n">
         <v>43416</v>
       </c>
       <c r="C115" s="1" t="s">
@@ -3022,11 +2868,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
-      <c r="A116" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="116">
+      <c r="A116" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="B116" s="2">
+      <c r="B116" s="5" t="n">
         <v>43444</v>
       </c>
       <c r="C116" s="1" t="s">
@@ -3036,11 +2882,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
-      <c r="A117" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="117">
+      <c r="A117" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="B117" s="7">
+      <c r="B117" s="6" t="n">
         <v>43476</v>
       </c>
       <c r="C117" s="1" t="s">
@@ -3050,14 +2896,16 @@
         <v>145</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="118">
+      <c r="B118" s="0"/>
+      <c r="C118" s="0"/>
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="1:4">
-      <c r="A119" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="119">
+      <c r="A119" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B119" s="2">
+      <c r="B119" s="5" t="n">
         <v>43507</v>
       </c>
       <c r="C119" s="1" t="s">
@@ -3067,11 +2915,11 @@
         <v>149</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
-      <c r="A120" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="120">
+      <c r="A120" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="B120" s="2">
+      <c r="B120" s="5" t="n">
         <v>43535</v>
       </c>
       <c r="C120" s="1" t="s">
@@ -3081,11 +2929,11 @@
         <v>149</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
-      <c r="A121" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="121">
+      <c r="A121" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B121" s="2">
+      <c r="B121" s="5" t="n">
         <v>43563</v>
       </c>
       <c r="C121" s="1" t="s">
@@ -3095,11 +2943,11 @@
         <v>149</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
-      <c r="A122" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="122">
+      <c r="A122" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="B122" s="2">
+      <c r="B122" s="5" t="n">
         <v>43598</v>
       </c>
       <c r="C122" s="1" t="s">
@@ -3109,11 +2957,11 @@
         <v>153</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
-      <c r="A123" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="123">
+      <c r="A123" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="B123" s="2">
+      <c r="B123" s="5" t="n">
         <v>43627</v>
       </c>
       <c r="C123" s="1" t="s">
@@ -3123,11 +2971,11 @@
         <v>153</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
-      <c r="A124" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="124">
+      <c r="A124" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="B124" s="2">
+      <c r="B124" s="5" t="n">
         <v>43654</v>
       </c>
       <c r="C124" s="1" t="s">
@@ -3137,11 +2985,11 @@
         <v>153</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
-      <c r="A125" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="125">
+      <c r="A125" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="B125" s="2">
+      <c r="B125" s="5" t="n">
         <v>43685</v>
       </c>
       <c r="C125" s="1" t="s">
@@ -3151,11 +2999,11 @@
         <v>157</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
-      <c r="A126" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="126">
+      <c r="A126" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B126" s="2">
+      <c r="B126" s="5" t="n">
         <v>43717</v>
       </c>
       <c r="C126" s="1" t="s">
@@ -3165,11 +3013,11 @@
         <v>157</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
-      <c r="A127" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="127">
+      <c r="A127" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="B127" s="2">
+      <c r="B127" s="5" t="n">
         <v>43747</v>
       </c>
       <c r="C127" s="1" t="s">
@@ -3179,11 +3027,11 @@
         <v>157</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
-      <c r="A128" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="128">
+      <c r="A128" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="B128" s="2">
+      <c r="B128" s="5" t="n">
         <v>43781</v>
       </c>
       <c r="C128" s="1" t="s">
@@ -3193,11 +3041,11 @@
         <v>161</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
-      <c r="A129" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="129">
+      <c r="A129" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B129" s="2">
+      <c r="B129" s="5" t="n">
         <v>43808</v>
       </c>
       <c r="C129" s="1" t="s">
@@ -3207,11 +3055,11 @@
         <v>161</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
-      <c r="A130" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="130">
+      <c r="A130" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B130" s="7">
+      <c r="B130" s="6" t="n">
         <v>43840</v>
       </c>
       <c r="C130" s="1" t="s">
@@ -3221,876 +3069,894 @@
         <v>161</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="131">
+      <c r="B131" s="0"/>
+      <c r="C131" s="0"/>
       <c r="D131" s="1"/>
     </row>
-    <row r="132" spans="1:4">
-      <c r="A132" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="132">
+      <c r="A132" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="B132" s="3"/>
-      <c r="C132" s="3"/>
+      <c r="B132" s="7"/>
+      <c r="C132" s="7"/>
       <c r="D132" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
-      <c r="A133" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="133">
+      <c r="A133" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="B133" s="3"/>
-      <c r="C133" s="3"/>
+      <c r="B133" s="7"/>
+      <c r="C133" s="7"/>
       <c r="D133" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
-      <c r="A134" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="134">
+      <c r="A134" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="B134" s="3"/>
-      <c r="C134" s="3"/>
+      <c r="B134" s="7"/>
+      <c r="C134" s="7"/>
       <c r="D134" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
-      <c r="A135" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="135">
+      <c r="A135" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="B135" s="3"/>
-      <c r="C135" s="3"/>
+      <c r="B135" s="7"/>
+      <c r="C135" s="7"/>
       <c r="D135" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
-      <c r="A136" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="136">
+      <c r="A136" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="B136" s="3"/>
-      <c r="C136" s="3"/>
+      <c r="B136" s="7"/>
+      <c r="C136" s="7"/>
       <c r="D136" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
-      <c r="A137" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="137">
+      <c r="A137" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="B137" s="3"/>
-      <c r="C137" s="3"/>
+      <c r="B137" s="7"/>
+      <c r="C137" s="7"/>
       <c r="D137" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
-      <c r="A138" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="138">
+      <c r="A138" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="B138" s="3"/>
-      <c r="C138" s="2">
+      <c r="B138" s="7"/>
+      <c r="C138" s="5" t="n">
         <v>44053</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
-      <c r="A139" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="139">
+      <c r="A139" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="B139" s="3"/>
-      <c r="C139" s="3"/>
+      <c r="B139" s="7"/>
+      <c r="C139" s="7"/>
       <c r="D139" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
-      <c r="A140" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="140">
+      <c r="A140" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="B140" s="3"/>
-      <c r="C140" s="2">
+      <c r="B140" s="7"/>
+      <c r="C140" s="5" t="n">
         <v>44112</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
-      <c r="A141" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="141">
+      <c r="A141" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="B141" s="3"/>
-      <c r="C141" s="2">
+      <c r="B141" s="7"/>
+      <c r="C141" s="5" t="n">
         <v>44144</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
-      <c r="A142" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="142">
+      <c r="A142" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="B142" s="3"/>
-      <c r="C142" s="2">
+      <c r="B142" s="7"/>
+      <c r="C142" s="5" t="n">
         <v>44179</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
-      <c r="A143" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="143">
+      <c r="A143" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B143" s="5">
-        <v>44209</v>
-      </c>
-      <c r="C143" s="5">
-        <v>44209</v>
-      </c>
+      <c r="B143" s="8"/>
+      <c r="C143" s="8"/>
       <c r="D143" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
-      <c r="A145" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="144">
+      <c r="B144" s="0"/>
+      <c r="C144" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="145">
+      <c r="A145" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="B145" s="2">
+      <c r="B145" s="5" t="n">
         <v>44236</v>
       </c>
-      <c r="C145" s="2">
+      <c r="C145" s="5" t="n">
         <v>44236</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
-      <c r="A146" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="146">
+      <c r="A146" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="B146" s="2">
+      <c r="B146" s="5" t="n">
         <v>44263</v>
       </c>
-      <c r="C146" s="2">
+      <c r="C146" s="5" t="n">
         <v>44263</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
-      <c r="A147" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="147">
+      <c r="A147" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="B147" s="3"/>
-      <c r="C147" s="2">
+      <c r="B147" s="7"/>
+      <c r="C147" s="5" t="n">
         <v>44298</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
-      <c r="A148" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="148">
+      <c r="A148" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B148" s="2">
+      <c r="B148" s="5" t="n">
         <v>44326</v>
       </c>
-      <c r="C148" s="2">
+      <c r="C148" s="5" t="n">
         <v>44326</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
-      <c r="A149" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="149">
+      <c r="A149" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="B149" s="2">
+      <c r="B149" s="5" t="n">
         <v>44361</v>
       </c>
-      <c r="C149" s="2">
+      <c r="C149" s="5" t="n">
         <v>44361</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
-      <c r="A150" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="150">
+      <c r="A150" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B150" s="3"/>
-      <c r="C150" s="2">
+      <c r="B150" s="7"/>
+      <c r="C150" s="5" t="n">
         <v>44384</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
-      <c r="A151" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="151">
+      <c r="A151" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="B151" s="2">
+      <c r="B151" s="5" t="n">
         <v>44417</v>
       </c>
-      <c r="C151" s="2">
+      <c r="C151" s="5" t="n">
         <v>44417</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
-      <c r="A152" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="152">
+      <c r="A152" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="B152" s="2">
+      <c r="B152" s="5" t="n">
         <v>44452</v>
       </c>
-      <c r="C152" s="2">
+      <c r="C152" s="5" t="n">
         <v>44452</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
-      <c r="A153" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="153">
+      <c r="A153" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="B153" s="2">
+      <c r="B153" s="5" t="n">
         <v>44480</v>
       </c>
-      <c r="C153" s="2">
+      <c r="C153" s="5" t="n">
         <v>44480</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
-      <c r="A154" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="154">
+      <c r="A154" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="B154" s="2">
+      <c r="B154" s="5" t="n">
         <v>44508</v>
       </c>
-      <c r="C154" s="2">
+      <c r="C154" s="5" t="n">
         <v>44508</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
-      <c r="A155" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="155">
+      <c r="A155" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="B155" s="3"/>
-      <c r="C155" s="2">
+      <c r="B155" s="7"/>
+      <c r="C155" s="5" t="n">
         <v>44537</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
-      <c r="A156" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="156">
+      <c r="A156" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="B156" s="2">
+      <c r="B156" s="5" t="n">
         <v>44572</v>
       </c>
-      <c r="C156" s="2">
+      <c r="C156" s="5" t="n">
         <v>44572</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
-      <c r="A158" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="157">
+      <c r="B157" s="0"/>
+      <c r="C157" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="158">
+      <c r="A158" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="B158" s="3"/>
-      <c r="C158" s="2">
+      <c r="B158" s="7"/>
+      <c r="C158" s="5" t="n">
         <v>44602</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
-      <c r="A159" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="159">
+      <c r="A159" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="B159" s="2">
+      <c r="B159" s="5" t="n">
         <v>44633</v>
       </c>
-      <c r="C159" s="2">
+      <c r="C159" s="5" t="n">
         <v>44633</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
-      <c r="A160" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="160">
+      <c r="A160" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B160" s="2">
+      <c r="B160" s="5" t="n">
         <v>44663</v>
       </c>
-      <c r="C160" s="2">
+      <c r="C160" s="5" t="n">
         <v>44663</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
-      <c r="A161" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="161">
+      <c r="A161" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="B161" s="3"/>
-      <c r="C161" s="2">
+      <c r="B161" s="7"/>
+      <c r="C161" s="5" t="n">
         <v>44692</v>
       </c>
       <c r="D161" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
-      <c r="A162" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="162">
+      <c r="A162" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="B162" s="3"/>
-      <c r="C162" s="2">
+      <c r="B162" s="7"/>
+      <c r="C162" s="5" t="n">
         <v>44726</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="163" spans="1:4">
-      <c r="A163" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="163">
+      <c r="A163" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="B163" s="3"/>
-      <c r="C163" s="2">
+      <c r="B163" s="7"/>
+      <c r="C163" s="5" t="n">
         <v>44754</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
-      <c r="A164" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="164">
+      <c r="A164" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="B164" s="3"/>
-      <c r="C164" s="2">
+      <c r="B164" s="7"/>
+      <c r="C164" s="5" t="n">
         <v>44782</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="165" spans="1:4">
-      <c r="A165" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="165">
+      <c r="A165" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="B165" s="3"/>
-      <c r="C165" s="2">
+      <c r="B165" s="7"/>
+      <c r="C165" s="5" t="n">
         <v>44812</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
-      <c r="A166" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="166">
+      <c r="A166" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="B166" s="3"/>
-      <c r="C166" s="2">
+      <c r="B166" s="7"/>
+      <c r="C166" s="5" t="n">
         <v>44844</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
-      <c r="A167" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="167">
+      <c r="A167" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="B167" s="3"/>
-      <c r="C167" s="2">
+      <c r="B167" s="7"/>
+      <c r="C167" s="5" t="n">
         <v>44874</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
-      <c r="A168" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="168">
+      <c r="A168" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="B168" s="3"/>
-      <c r="C168" s="2">
+      <c r="B168" s="7"/>
+      <c r="C168" s="5" t="n">
         <v>44903</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="169" spans="1:4">
-      <c r="A169" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="169">
+      <c r="A169" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="B169" s="3"/>
-      <c r="C169" s="2">
+      <c r="B169" s="7"/>
+      <c r="C169" s="5" t="n">
         <v>44937</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
-      <c r="A171" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="170">
+      <c r="B170" s="0"/>
+      <c r="C170" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="171">
+      <c r="A171" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="B171" s="3"/>
-      <c r="C171" s="2">
+      <c r="B171" s="7"/>
+      <c r="C171" s="5" t="n">
         <v>44965</v>
       </c>
       <c r="D171" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
-      <c r="A172" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="172">
+      <c r="A172" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="B172" s="3"/>
-      <c r="C172" s="2">
+      <c r="B172" s="7"/>
+      <c r="C172" s="5" t="n">
         <v>44993</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
-      <c r="A173" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="173">
+      <c r="A173" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="B173" s="3"/>
-      <c r="C173" s="2">
+      <c r="B173" s="7"/>
+      <c r="C173" s="5" t="n">
         <v>45027</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="174" spans="1:4">
-      <c r="A174" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="174">
+      <c r="A174" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="B174" s="3"/>
-      <c r="C174" s="2">
+      <c r="B174" s="7"/>
+      <c r="C174" s="5" t="n">
         <v>45056</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
-      <c r="A175" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="175">
+      <c r="A175" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="B175" s="3"/>
-      <c r="C175" s="2">
+      <c r="B175" s="7"/>
+      <c r="C175" s="5" t="n">
         <v>45085</v>
       </c>
       <c r="D175" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
-      <c r="A176" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="176">
+      <c r="A176" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B176" s="3"/>
-      <c r="C176" s="2">
+      <c r="B176" s="7"/>
+      <c r="C176" s="5" t="n">
         <v>45117</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
-      <c r="A177" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="177">
+      <c r="A177" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="B177" s="3"/>
-      <c r="C177" s="2">
+      <c r="B177" s="7"/>
+      <c r="C177" s="5" t="n">
         <v>45147</v>
       </c>
       <c r="D177" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="178" spans="1:4">
-      <c r="A178" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="178">
+      <c r="A178" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="B178" s="3"/>
-      <c r="C178" s="2">
+      <c r="B178" s="7"/>
+      <c r="C178" s="5" t="n">
         <v>45181</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="179" spans="1:4">
-      <c r="A179" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="179">
+      <c r="A179" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="B179" s="2">
+      <c r="B179" s="5" t="n">
         <v>45208</v>
       </c>
-      <c r="C179" s="2">
+      <c r="C179" s="5" t="n">
         <v>45208</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="180" spans="1:4">
-      <c r="A180" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="180">
+      <c r="A180" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="B180" s="2">
+      <c r="B180" s="5" t="n">
         <v>45238</v>
       </c>
-      <c r="C180" s="2">
+      <c r="C180" s="5" t="n">
         <v>45238</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="181" spans="1:4">
-      <c r="A181" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="181">
+      <c r="A181" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="B181" s="2">
+      <c r="B181" s="5" t="n">
         <v>45271</v>
       </c>
-      <c r="C181" s="2">
+      <c r="C181" s="5" t="n">
         <v>45271</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="182" spans="1:4">
-      <c r="A182" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="182">
+      <c r="A182" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="B182" s="2">
+      <c r="B182" s="5" t="n">
         <v>45301</v>
       </c>
-      <c r="C182" s="2">
+      <c r="C182" s="5" t="n">
         <v>45301</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="184" spans="1:4">
-      <c r="A184" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="183">
+      <c r="B183" s="0"/>
+      <c r="C183" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="184">
+      <c r="A184" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B184" s="2">
+      <c r="B184" s="5" t="n">
         <v>45330</v>
       </c>
-      <c r="C184" s="2">
+      <c r="C184" s="5" t="n">
         <v>45330</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="185" spans="1:4">
-      <c r="A185" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="185">
+      <c r="A185" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="B185" s="2">
+      <c r="B185" s="5" t="n">
         <v>45363</v>
       </c>
-      <c r="C185" s="2">
+      <c r="C185" s="5" t="n">
         <v>45363</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="186" spans="1:4">
-      <c r="A186" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="186">
+      <c r="A186" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="B186" s="2">
+      <c r="B186" s="5" t="n">
         <v>45393</v>
       </c>
-      <c r="C186" s="2">
+      <c r="C186" s="5" t="n">
         <v>45393</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="187" spans="1:4">
-      <c r="A187" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="187">
+      <c r="A187" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="B187" s="2">
+      <c r="B187" s="5" t="n">
         <v>45426</v>
       </c>
-      <c r="C187" s="2">
+      <c r="C187" s="5" t="n">
         <v>45426</v>
       </c>
       <c r="D187" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="188" spans="1:4">
-      <c r="A188" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="188">
+      <c r="A188" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="B188" s="2">
+      <c r="B188" s="5" t="n">
         <v>45454</v>
       </c>
-      <c r="C188" s="2">
+      <c r="C188" s="5" t="n">
         <v>45454</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="15">
-      <c r="A189" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="189">
+      <c r="A189" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="B189" s="2">
+      <c r="B189" s="5" t="n">
         <v>45483</v>
       </c>
-      <c r="C189" s="9">
+      <c r="C189" s="9" t="n">
         <v>45483</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="190" spans="1:4">
-      <c r="A190" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="190">
+      <c r="A190" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="B190" s="2">
+      <c r="B190" s="5" t="n">
         <v>45513</v>
       </c>
-      <c r="C190" s="2">
+      <c r="C190" s="5" t="n">
         <v>45513</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="191" spans="1:4">
-      <c r="A191" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="191">
+      <c r="A191" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="B191" s="4"/>
-      <c r="C191" s="2">
+      <c r="B191" s="3"/>
+      <c r="C191" s="5" t="n">
         <v>45545</v>
       </c>
       <c r="D191" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="192" spans="1:4">
-      <c r="A192" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="192">
+      <c r="A192" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="B192" s="2">
+      <c r="B192" s="5" t="n">
         <v>45573</v>
       </c>
-      <c r="C192" s="2">
+      <c r="C192" s="5" t="n">
         <v>45573</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="193" spans="1:4">
-      <c r="A193" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="193">
+      <c r="A193" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="B193" s="2">
+      <c r="B193" s="5" t="n">
         <v>45608</v>
       </c>
-      <c r="C193" s="2">
+      <c r="C193" s="5" t="n">
         <v>45608</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="194" spans="1:4">
-      <c r="A194" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="194">
+      <c r="A194" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="B194" s="2">
+      <c r="B194" s="5" t="n">
         <v>45636</v>
       </c>
-      <c r="C194" s="2">
+      <c r="C194" s="5" t="n">
         <v>45636</v>
       </c>
       <c r="D194" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="195" spans="1:4">
-      <c r="A195" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="195">
+      <c r="A195" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B195" s="2">
+      <c r="B195" s="5" t="n">
         <v>45670</v>
       </c>
-      <c r="C195" s="2">
+      <c r="C195" s="5" t="n">
         <v>45670</v>
       </c>
       <c r="D195" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="196" spans="1:4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="196">
+      <c r="C196" s="0"/>
       <c r="D196" s="1"/>
     </row>
-    <row r="198" spans="1:4">
-      <c r="A198" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="197">
+      <c r="C197" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="198">
+      <c r="A198" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="C198" s="2">
+      <c r="C198" s="5" t="n">
         <v>45699</v>
       </c>
       <c r="D198" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="199" spans="1:4">
-      <c r="A199" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="199">
+      <c r="A199" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="C199" s="2">
+      <c r="C199" s="5" t="n">
         <v>45728</v>
       </c>
       <c r="D199" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="200" spans="1:4">
-      <c r="A200" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="200">
+      <c r="A200" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="C200" s="2">
+      <c r="C200" s="5" t="n">
         <v>45755</v>
       </c>
       <c r="D200" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="201" spans="1:4">
-      <c r="A201" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="201">
+      <c r="A201" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="C201" s="2">
+      <c r="C201" s="5" t="n">
         <v>45790</v>
       </c>
       <c r="D201" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="202" spans="1:4">
-      <c r="A202" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="202">
+      <c r="A202" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="C202" s="2">
+      <c r="C202" s="5" t="n">
         <v>45819</v>
       </c>
       <c r="D202" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="203" spans="1:4">
-      <c r="A203" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="203">
+      <c r="A203" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="C203" s="2">
+      <c r="C203" s="5" t="n">
         <v>45847</v>
       </c>
       <c r="D203" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="204" spans="1:4">
-      <c r="A204" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="204">
+      <c r="A204" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="C204" s="2">
+      <c r="C204" s="5" t="n">
         <v>45880</v>
       </c>
       <c r="D204" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="205" spans="1:4">
-      <c r="A205" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="205">
+      <c r="A205" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="C205" s="2">
+      <c r="C205" s="5" t="n">
         <v>45909</v>
       </c>
       <c r="D205" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="206" spans="1:4">
-      <c r="A206" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="206">
+      <c r="A206" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="C206" s="2">
+      <c r="C206" s="5" t="n">
         <v>45939</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="207" spans="1:4">
-      <c r="A207" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="207">
+      <c r="A207" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="C207" s="2">
+      <c r="C207" s="5" t="n">
         <v>45973</v>
       </c>
       <c r="D207" s="1" t="s">
@@ -4098,7 +3964,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>